<commit_message>
wsr updated, and small changes
</commit_message>
<xml_diff>
--- a/dataSources/WSR/ACCOUNT_MASTER.xlsx
+++ b/dataSources/WSR/ACCOUNT_MASTER.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27321"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VigneshD\repository\vsCode\qaDash\dataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VigneshD\repository\vsCode\KMDV-Dash\dataSources\WSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{0F8C332E-20C7-4FE6-8FBC-D589C740ED26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04AD3E11-27B6-4573-B944-BB9933E9CF03}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9D9989-0F5F-42DD-9D49-4EF00F3B0533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="53">
   <si>
     <t>Task Name</t>
   </si>
@@ -96,18 +96,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Week Data Type</t>
-  </si>
-  <si>
-    <t>Week Count</t>
-  </si>
-  <si>
-    <t>Project Metrics</t>
-  </si>
-  <si>
-    <t>Total Count</t>
-  </si>
-  <si>
     <t>Testcase preparation</t>
   </si>
   <si>
@@ -123,12 +111,6 @@
     <t>No defect logged for the week</t>
   </si>
   <si>
-    <t>Manual created</t>
-  </si>
-  <si>
-    <t>Total manual</t>
-  </si>
-  <si>
     <t>Meetings</t>
   </si>
   <si>
@@ -138,12 +120,6 @@
     <t>Test case preparation for To Maintain Sheel Legal Entity screen</t>
   </si>
   <si>
-    <t>Manual execution</t>
-  </si>
-  <si>
-    <t>Total manual execution</t>
-  </si>
-  <si>
     <t>Review the testcase</t>
   </si>
   <si>
@@ -153,40 +129,19 @@
     <t>Test case preparation for Create Legal Entity Relationship- Internal Entity screen</t>
   </si>
   <si>
-    <t>Automation created</t>
-  </si>
-  <si>
-    <t>Total automation</t>
-  </si>
-  <si>
     <t>Vignesh</t>
   </si>
   <si>
     <t>Test case preparation for Create Legal Entity Relationship- External Entity screen</t>
   </si>
   <si>
-    <t>Automation execution</t>
-  </si>
-  <si>
-    <t>Total automation execution</t>
-  </si>
-  <si>
     <t>Test case preparation for View Legal Entities Relationships List screen</t>
-  </si>
-  <si>
-    <t>Bugs Identified</t>
-  </si>
-  <si>
-    <t>Total bugs</t>
   </si>
   <si>
     <t>Test case preparation for
 View Legal Entities List screen</t>
   </si>
   <si>
-    <t>Automation coverage %</t>
-  </si>
-  <si>
     <t>Test case preparation for View Legal Entities List (v.2) screen</t>
   </si>
   <si>
@@ -212,13 +167,43 @@
   </si>
   <si>
     <t>Testcase review</t>
+  </si>
+  <si>
+    <t>Activity This Week</t>
+  </si>
+  <si>
+    <t>Manual test cases created</t>
+  </si>
+  <si>
+    <t>Manual test cases conducted</t>
+  </si>
+  <si>
+    <t>Automation test cases created</t>
+  </si>
+  <si>
+    <t>Automation test cases processed</t>
+  </si>
+  <si>
+    <t>Bugs identified</t>
+  </si>
+  <si>
+    <t>Project Metrics Since Inception</t>
+  </si>
+  <si>
+    <t>Automation coverage</t>
+  </si>
+  <si>
+    <t>Count.</t>
+  </si>
+  <si>
+    <t>Count..</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,14 +250,6 @@
       <name val="Aptos"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -368,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -423,7 +400,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,39 +683,41 @@
   <dimension ref="A1:AC18"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+      <selection activeCell="Y1" sqref="Y1:AC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="73.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="2"/>
-    <col min="12" max="12" width="89.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="2"/>
-    <col min="18" max="18" width="65.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="2"/>
+    <col min="4" max="4" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="2"/>
+    <col min="7" max="7" width="73.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="2"/>
+    <col min="12" max="12" width="89.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="2"/>
+    <col min="18" max="18" width="65.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="8.88671875" style="2"/>
+    <col min="28" max="28" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -798,47 +776,47 @@
         <v>18</v>
       </c>
       <c r="Y1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A2" s="20" t="s">
         <v>19</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" ht="30.75">
-      <c r="A2" s="20" t="s">
-        <v>23</v>
       </c>
       <c r="B2" s="4">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I2" s="16">
         <v>45566</v>
       </c>
       <c r="J2" s="17"/>
       <c r="L2" s="14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N2" s="16">
         <v>45566</v>
@@ -846,55 +824,55 @@
       <c r="O2" s="17"/>
       <c r="P2" s="11"/>
       <c r="R2" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
-      <c r="Y2" s="6" t="s">
-        <v>28</v>
+      <c r="Y2" t="s">
+        <v>44</v>
       </c>
       <c r="Z2" s="10">
         <v>50</v>
       </c>
       <c r="AA2" s="11"/>
-      <c r="AB2" s="6" t="s">
-        <v>29</v>
+      <c r="AB2" t="s">
+        <v>44</v>
       </c>
       <c r="AC2" s="10">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E3" s="4">
         <v>1.5</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I3" s="16">
         <v>45566</v>
       </c>
       <c r="J3" s="17"/>
       <c r="L3" s="14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N3" s="16">
         <v>45566</v>
@@ -906,48 +884,48 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-      <c r="Y3" s="6" t="s">
-        <v>33</v>
+      <c r="Y3" t="s">
+        <v>45</v>
       </c>
       <c r="Z3" s="10">
         <v>0</v>
       </c>
       <c r="AA3" s="11"/>
-      <c r="AB3" s="6" t="s">
-        <v>34</v>
+      <c r="AB3" t="s">
+        <v>45</v>
       </c>
       <c r="AC3" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A4" s="20" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4">
         <v>0.5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E4" s="4">
         <v>5</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I4" s="16">
         <v>45566</v>
       </c>
       <c r="J4" s="17"/>
       <c r="L4" s="18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N4" s="16">
         <v>45566</v>
@@ -959,44 +937,44 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-      <c r="Y4" s="6" t="s">
-        <v>38</v>
+      <c r="Y4" t="s">
+        <v>46</v>
       </c>
       <c r="Z4" s="10">
         <v>0</v>
       </c>
       <c r="AA4" s="11"/>
-      <c r="AB4" s="6" t="s">
-        <v>39</v>
+      <c r="AB4" t="s">
+        <v>46</v>
       </c>
       <c r="AC4" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I5" s="16">
         <v>45566</v>
       </c>
       <c r="J5" s="17"/>
       <c r="L5" s="18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N5" s="16">
         <v>45566</v>
@@ -1008,36 +986,36 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
-      <c r="Y5" s="6" t="s">
-        <v>42</v>
+      <c r="Y5" t="s">
+        <v>47</v>
       </c>
       <c r="Z5" s="10">
         <v>0</v>
       </c>
       <c r="AA5" s="11"/>
-      <c r="AB5" s="6" t="s">
-        <v>43</v>
+      <c r="AB5" t="s">
+        <v>47</v>
       </c>
       <c r="AC5" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="16.8" x14ac:dyDescent="0.4">
       <c r="G6" s="18" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I6" s="16">
         <v>45566</v>
       </c>
       <c r="J6" s="17"/>
       <c r="L6" s="18" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N6" s="16">
         <v>45566</v>
@@ -1049,36 +1027,36 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
-      <c r="Y6" s="6" t="s">
-        <v>45</v>
+      <c r="Y6" t="s">
+        <v>48</v>
       </c>
       <c r="Z6" s="10">
         <v>0</v>
       </c>
       <c r="AA6" s="11"/>
-      <c r="AB6" s="6" t="s">
-        <v>46</v>
+      <c r="AB6" t="s">
+        <v>48</v>
       </c>
       <c r="AC6" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" ht="30" x14ac:dyDescent="0.4">
       <c r="G7" s="18" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I7" s="16">
         <v>45566</v>
       </c>
       <c r="J7" s="17"/>
       <c r="L7" s="18" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N7" s="16">
         <v>45566</v>
@@ -1093,29 +1071,29 @@
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
       <c r="AA7" s="11"/>
-      <c r="AB7" s="6" t="s">
-        <v>48</v>
+      <c r="AB7" t="s">
+        <v>50</v>
       </c>
       <c r="AC7" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="30.75">
+    <row r="8" spans="1:29" ht="16.8" x14ac:dyDescent="0.4">
       <c r="G8" s="18" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I8" s="16">
         <v>45566</v>
       </c>
       <c r="J8" s="17"/>
       <c r="L8" s="18" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N8" s="16">
         <v>45566</v>
@@ -1130,22 +1108,22 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:29" ht="30.75">
+    <row r="9" spans="1:29" ht="16.8" x14ac:dyDescent="0.4">
       <c r="G9" s="18" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I9" s="16">
         <v>45566</v>
       </c>
       <c r="J9" s="19"/>
       <c r="L9" s="18" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N9" s="16">
         <v>45566</v>
@@ -1160,16 +1138,16 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:29" ht="30.75">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G10"/>
       <c r="H10"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="L10" s="18" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N10" s="16">
         <v>45566</v>
@@ -1182,7 +1160,7 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="L11"/>
       <c r="M11"/>
       <c r="N11"/>
@@ -1194,7 +1172,7 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
@@ -1202,7 +1180,7 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -1210,7 +1188,7 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
@@ -1218,7 +1196,7 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -1226,7 +1204,7 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -1234,7 +1212,7 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="18:23">
+    <row r="17" spans="18:23" x14ac:dyDescent="0.3">
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -1242,7 +1220,7 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
     </row>
-    <row r="18" spans="18:23">
+    <row r="18" spans="18:23" x14ac:dyDescent="0.3">
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
@@ -1260,39 +1238,41 @@
   <dimension ref="A1:AC18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="73.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="2"/>
-    <col min="12" max="12" width="89.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="2"/>
-    <col min="17" max="17" width="8.85546875" style="2"/>
-    <col min="18" max="18" width="65.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="2"/>
+    <col min="4" max="4" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="2"/>
+    <col min="7" max="7" width="73.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="2"/>
+    <col min="12" max="12" width="89.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="2"/>
+    <col min="17" max="17" width="8.88671875" style="2"/>
+    <col min="18" max="18" width="65.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="8.88671875" style="2"/>
+    <col min="28" max="28" width="28.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1351,91 +1331,91 @@
         <v>18</v>
       </c>
       <c r="Y1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="32.4" x14ac:dyDescent="0.4">
+      <c r="A2" s="23" t="s">
         <v>19</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" ht="30.75">
-      <c r="A2" s="23" t="s">
-        <v>23</v>
       </c>
       <c r="B2" s="4">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
       <c r="L2" s="21" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="12"/>
       <c r="R2" s="13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
-      <c r="Y2" s="6" t="s">
-        <v>28</v>
+      <c r="Y2" t="s">
+        <v>44</v>
       </c>
       <c r="Z2" s="10">
         <v>6</v>
       </c>
       <c r="AA2" s="11"/>
-      <c r="AB2" s="6" t="s">
-        <v>29</v>
+      <c r="AB2" t="s">
+        <v>44</v>
       </c>
       <c r="AC2" s="10">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="32.4" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B3" s="4">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E3" s="4">
         <v>3</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -1450,38 +1430,38 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-      <c r="Y3" s="6" t="s">
-        <v>33</v>
+      <c r="Y3" t="s">
+        <v>45</v>
       </c>
       <c r="Z3" s="10">
         <v>0</v>
       </c>
       <c r="AA3" s="11"/>
-      <c r="AB3" s="6" t="s">
-        <v>34</v>
+      <c r="AB3" t="s">
+        <v>45</v>
       </c>
       <c r="AC3" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="32.4" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E4" s="4">
         <v>5</v>
       </c>
       <c r="G4" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="22" t="s">
         <v>37</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>52</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
@@ -1496,34 +1476,34 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-      <c r="Y4" s="6" t="s">
-        <v>38</v>
+      <c r="Y4" t="s">
+        <v>46</v>
       </c>
       <c r="Z4" s="10">
         <v>0</v>
       </c>
       <c r="AA4" s="11"/>
-      <c r="AB4" s="6" t="s">
-        <v>39</v>
+      <c r="AB4" t="s">
+        <v>46</v>
       </c>
       <c r="AC4" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
@@ -1538,21 +1518,21 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
-      <c r="Y5" s="6" t="s">
-        <v>42</v>
+      <c r="Y5" t="s">
+        <v>47</v>
       </c>
       <c r="Z5" s="10">
         <v>0</v>
       </c>
       <c r="AA5" s="11"/>
-      <c r="AB5" s="6" t="s">
-        <v>43</v>
+      <c r="AB5" t="s">
+        <v>47</v>
       </c>
       <c r="AC5" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1564,21 +1544,21 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
-      <c r="Y6" s="6" t="s">
-        <v>45</v>
+      <c r="Y6" t="s">
+        <v>48</v>
       </c>
       <c r="Z6" s="10">
         <v>0</v>
       </c>
       <c r="AA6" s="11"/>
-      <c r="AB6" s="6" t="s">
-        <v>46</v>
+      <c r="AB6" t="s">
+        <v>48</v>
       </c>
       <c r="AC6" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q7" s="12"/>
       <c r="R7" s="13"/>
       <c r="S7" s="1"/>
@@ -1589,14 +1569,14 @@
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
       <c r="AA7" s="11"/>
-      <c r="AB7" s="6" t="s">
-        <v>48</v>
+      <c r="AB7" t="s">
+        <v>50</v>
       </c>
       <c r="AC7" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q8" s="12"/>
       <c r="R8" s="13"/>
       <c r="S8" s="1"/>
@@ -1607,7 +1587,7 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q9" s="12"/>
       <c r="R9" s="13"/>
       <c r="S9" s="1"/>
@@ -1618,7 +1598,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q10" s="12"/>
       <c r="R10" s="13"/>
       <c r="S10" s="1"/>
@@ -1627,7 +1607,7 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q11" s="12"/>
       <c r="R11" s="13"/>
       <c r="S11" s="1"/>
@@ -1636,7 +1616,7 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q12" s="12"/>
       <c r="R12" s="13"/>
       <c r="S12" s="1"/>
@@ -1645,7 +1625,7 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q13" s="12"/>
       <c r="R13" s="13"/>
       <c r="S13" s="1"/>
@@ -1654,7 +1634,7 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q14" s="12"/>
       <c r="R14" s="13"/>
       <c r="S14" s="1"/>
@@ -1663,7 +1643,7 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q15" s="12"/>
       <c r="R15" s="13"/>
       <c r="S15" s="1"/>
@@ -1672,7 +1652,7 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -1680,7 +1660,7 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="18:23">
+    <row r="17" spans="18:23" x14ac:dyDescent="0.3">
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -1688,7 +1668,7 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
     </row>
-    <row r="18" spans="18:23">
+    <row r="18" spans="18:23" x14ac:dyDescent="0.3">
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
@@ -1702,6 +1682,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000215C4F9D57D37439F8ACEF5C886EA75" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0c845befd03cfebab38c352a41d34e6a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2a5c4c29-2a22-48a5-946d-f6132279c68c" xmlns:ns3="46e2485f-814c-41c1-b1d1-92fb45bc36b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba1163b5c6633ba9dadda0673900e477" ns2:_="" ns3:_="">
     <xsd:import namespace="2a5c4c29-2a22-48a5-946d-f6132279c68c"/>
@@ -1878,29 +1873,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{481829E1-7F78-46F9-BDB6-11979196389B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6474CE3A-0E71-4669-84F6-F58852B7165A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4456B1F5-8C68-4690-8976-0268561EDD0D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4456B1F5-8C68-4690-8976-0268561EDD0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6474CE3A-0E71-4669-84F6-F58852B7165A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{481829E1-7F78-46F9-BDB6-11979196389B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2a5c4c29-2a22-48a5-946d-f6132279c68c"/>
+    <ds:schemaRef ds:uri="46e2485f-814c-41c1-b1d1-92fb45bc36b1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>